<commit_message>
Finished batch insert data akun mhs
</commit_message>
<xml_diff>
--- a/public/documents/data-mhs/DataMhs.xlsx
+++ b/public/documents/data-mhs/DataMhs.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="350">
   <si>
     <t>nim</t>
   </si>
@@ -36,7 +34,7 @@
     <t>LABIB HABIBIE SANJAYA</t>
   </si>
   <si>
-    <t>196511071992031000</t>
+    <t>196511071992031001</t>
   </si>
   <si>
     <t>24060120120006</t>
@@ -45,7 +43,7 @@
     <t>NADIATUS SALAM</t>
   </si>
   <si>
-    <t>197308291998022000</t>
+    <t>196511071992031002</t>
   </si>
   <si>
     <t>24060120120009</t>
@@ -54,13 +52,16 @@
     <t>SHABRINA AZIZNY</t>
   </si>
   <si>
+    <t>196511071992031003</t>
+  </si>
+  <si>
     <t>24060120120012</t>
   </si>
   <si>
     <t>ADINDA DESTIFANY ZENNIAR</t>
   </si>
   <si>
-    <t>197007051997021000</t>
+    <t>197007051997021001</t>
   </si>
   <si>
     <t>24060120120015</t>
@@ -69,7 +70,7 @@
     <t>WASIS PAMBUDI</t>
   </si>
   <si>
-    <t>197108111997021000</t>
+    <t>197108111997021004</t>
   </si>
   <si>
     <t>24060120120018</t>
@@ -78,13 +79,16 @@
     <t>WAHYU ARIF MAULANA</t>
   </si>
   <si>
+    <t>197308291998022001</t>
+  </si>
+  <si>
     <t>24060120120021</t>
   </si>
   <si>
     <t>AGNES TRIANA CYNTIANESA</t>
   </si>
   <si>
-    <t>197601102009122000</t>
+    <t>197601102009122002</t>
   </si>
   <si>
     <t>24060120120024</t>
@@ -93,7 +97,7 @@
     <t>MAYA NURUL NIKMAH</t>
   </si>
   <si>
-    <t>197805022005012000</t>
+    <t>197805022005012002</t>
   </si>
   <si>
     <t>24060120120027</t>
@@ -102,7 +106,7 @@
     <t>NADYA MUMTAZAH</t>
   </si>
   <si>
-    <t>197805162003121000</t>
+    <t>197805162003121001</t>
   </si>
   <si>
     <t>24060120120030</t>
@@ -111,7 +115,7 @@
     <t>ZARA ZETIRA PUTI</t>
   </si>
   <si>
-    <t>197902122008121000</t>
+    <t>197902122008121002</t>
   </si>
   <si>
     <t>24060120120033</t>
@@ -120,7 +124,7 @@
     <t>ARIFA ALIF MALICHA KHAIRUNNISA</t>
   </si>
   <si>
-    <t>197905242009121000</t>
+    <t>19790524200912100</t>
   </si>
   <si>
     <t>24060120130039</t>
@@ -129,7 +133,7 @@
     <t>HIKMAL ARKAN NUR ZAIDAN</t>
   </si>
   <si>
-    <t>197907202003121000</t>
+    <t>197907202003121002</t>
   </si>
   <si>
     <t>24060120130054</t>
@@ -138,7 +142,7 @@
     <t>AULIA CHAIRUNISA PUTRI</t>
   </si>
   <si>
-    <t>198009142006041000</t>
+    <t>198009142006041002</t>
   </si>
   <si>
     <t>24060120130063</t>
@@ -147,7 +151,7 @@
     <t>BINTANG ARYO BIMO WINANDA</t>
   </si>
   <si>
-    <t>198010212005011000</t>
+    <t>198010212005011003</t>
   </si>
   <si>
     <t>24060120130069</t>
@@ -156,7 +160,7 @@
     <t>HAMID ALBAR NURRASYID</t>
   </si>
   <si>
-    <t>198012272015041000</t>
+    <t>198012272015041002</t>
   </si>
   <si>
     <t>24060120130072</t>
@@ -165,7 +169,7 @@
     <t>R. DAMANHURI</t>
   </si>
   <si>
-    <t>198104202005012000</t>
+    <t>198104202005012001</t>
   </si>
   <si>
     <t>24060120130081</t>
@@ -174,7 +178,7 @@
     <t>ARJUNA WAHYU KUSUMA</t>
   </si>
   <si>
-    <t>198104212008121000</t>
+    <t>198104212008121002</t>
   </si>
   <si>
     <t>24060120130087</t>
@@ -183,7 +187,7 @@
     <t>FAJAR IVANO GAMAWAN</t>
   </si>
   <si>
-    <t>198106202015041000</t>
+    <t>198106202015041002</t>
   </si>
   <si>
     <t>24060120130114</t>
@@ -192,7 +196,7 @@
     <t>ALFIAN PUTRA SETYAWAN</t>
   </si>
   <si>
-    <t>198302032006041000</t>
+    <t>198302032006041002</t>
   </si>
   <si>
     <t>24060120130117</t>
@@ -201,7 +205,7 @@
     <t>MUHAMMAD RAFLI AKBAR</t>
   </si>
   <si>
-    <t>198404112019031000</t>
+    <t>198404112019031009</t>
   </si>
   <si>
     <t>24060120130120</t>
@@ -210,7 +214,7 @@
     <t>AQSYA OCLIBEL ARFINIA</t>
   </si>
   <si>
-    <t>198511252018032000</t>
+    <t>198511252018032001</t>
   </si>
   <si>
     <t>24060120130123</t>
@@ -219,7 +223,7 @@
     <t>MUHAMMAD HAFIZH ROIHAN</t>
   </si>
   <si>
-    <t>198611050214011000</t>
+    <t>198611050214011680</t>
   </si>
   <si>
     <t>24060120130135</t>
@@ -228,7 +232,7 @@
     <t>MUHAMMAD RIFQI ZAIDAN</t>
   </si>
   <si>
-    <t>198803222020121000</t>
+    <t>198803222020121010</t>
   </si>
   <si>
     <t>24060120140036</t>
@@ -237,7 +241,7 @@
     <t>ADIP DWI SASONGKO</t>
   </si>
   <si>
-    <t>198903032015042000</t>
+    <t>198903032015042002</t>
   </si>
   <si>
     <t>24060120140042</t>
@@ -246,7 +250,7 @@
     <t>NOVIA DEWI MAHARANI</t>
   </si>
   <si>
-    <t>198911010214012000</t>
+    <t>198911010214012670</t>
   </si>
   <si>
     <t>24060120140045</t>
@@ -313,6 +317,9 @@
   </si>
   <si>
     <t>PUTRA FAJAR</t>
+  </si>
+  <si>
+    <t>197905242009121003</t>
   </si>
   <si>
     <t>24060120140099</t>
@@ -1791,7 +1798,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1821,7 +1828,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1829,6 +1835,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="32" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="top"/>
     </xf>
@@ -2210,18 +2217,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F176"/>
+  <dimension ref="A1:J176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="G162" sqref="G162"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24.3333333333333" customWidth="1"/>
     <col min="2" max="2" width="44.7777777777778" customWidth="1"/>
     <col min="3" max="3" width="10.7777777777778" customWidth="1"/>
     <col min="4" max="4" width="20.8888888888889" customWidth="1"/>
+    <col min="10" max="10" width="20.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.15" spans="1:4">
@@ -2249,7 +2257,7 @@
         <f ca="1" t="shared" ref="C2:C65" si="0">IF(MID(A2,9,3)="120","SNMPTN",IF(MID(A2,9,3)="130","SBMPTN",IF(RAND()&lt;0.8,"Mandiri","Lainnya")))</f>
         <v>SNMPTN</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2264,7 +2272,7 @@
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="9"/>
@@ -2280,2454 +2288,2458 @@
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
+      <c r="D4" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
+      <c r="D5" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
+      <c r="D6" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
+      <c r="D7" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D8" t="s">
-        <v>22</v>
+      <c r="D8" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D9" t="s">
-        <v>25</v>
+      <c r="D9" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D10" t="s">
-        <v>28</v>
+      <c r="D10" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C12" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D12" t="s">
-        <v>34</v>
+      <c r="D12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" t="str">
+        <f>_xlfn.CONCAT("",K12)</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D13" t="s">
-        <v>37</v>
+      <c r="D13" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D14" t="s">
-        <v>40</v>
+      <c r="D14" s="14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C15" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D15" t="s">
-        <v>43</v>
+      <c r="D15" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C16" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D16" t="s">
-        <v>46</v>
+      <c r="D16" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C17" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D17" t="s">
-        <v>49</v>
+      <c r="D17" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C18" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D18" t="s">
-        <v>52</v>
+      <c r="D18" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C19" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D19" t="s">
-        <v>55</v>
+      <c r="D19" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D20" t="s">
-        <v>58</v>
+      <c r="D20" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C21" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D21" t="s">
-        <v>61</v>
+      <c r="D21" s="14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C22" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D22" t="s">
-        <v>64</v>
+      <c r="D22" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C23" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D23" t="s">
-        <v>67</v>
+      <c r="D23" s="14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C24" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D24" t="s">
-        <v>70</v>
+      <c r="D24" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C25" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D25" t="s">
-        <v>73</v>
+      <c r="D25" s="14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C26" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D26" t="s">
-        <v>76</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C27" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C28" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D28" t="s">
-        <v>6</v>
+      <c r="D28" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C29" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D29" t="s">
-        <v>6</v>
+      <c r="D29" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C30" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D30" t="s">
-        <v>14</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C31" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D31" t="s">
-        <v>17</v>
+      <c r="D31" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C32" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D32" t="s">
-        <v>9</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C33" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D33" t="s">
-        <v>22</v>
+      <c r="D33" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C34" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D34" t="s">
-        <v>25</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C35" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D35" t="s">
-        <v>28</v>
+      <c r="D35" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C36" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D36" t="s">
-        <v>31</v>
+      <c r="D36" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C37" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D37" t="s">
-        <v>34</v>
+      <c r="D37" s="14" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C38" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D38" t="s">
-        <v>37</v>
+      <c r="D38" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C39" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D39" t="s">
-        <v>40</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="7" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C40" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D40" t="s">
-        <v>43</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C41" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D41" t="s">
-        <v>46</v>
+      <c r="D41" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C42" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D42" t="s">
-        <v>49</v>
+      <c r="D42" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C43" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D43" t="s">
-        <v>52</v>
+      <c r="D43" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C44" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D44" t="s">
-        <v>55</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="7" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C45" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Lainnya</v>
       </c>
-      <c r="D45" t="s">
-        <v>58</v>
+      <c r="D45" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="7" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C46" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D46" t="s">
-        <v>61</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C47" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D47" t="s">
-        <v>64</v>
+      <c r="D47" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C48" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D48" t="s">
-        <v>67</v>
+      <c r="D48" s="14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C49" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D49" t="s">
-        <v>70</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C50" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D50" t="s">
-        <v>73</v>
+      <c r="D50" s="14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C51" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D51" t="s">
-        <v>76</v>
+      <c r="D51" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C52" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D52" t="s">
+        <v>Mandiri</v>
+      </c>
+      <c r="D52" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C53" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D53" t="s">
-        <v>6</v>
+      <c r="D53" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C54" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D54" t="s">
-        <v>6</v>
+      <c r="D54" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C55" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>Mandiri</v>
       </c>
-      <c r="D55" t="s">
-        <v>14</v>
+      <c r="D55" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C56" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D56" t="s">
-        <v>17</v>
+      <c r="D56" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C57" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D57" t="s">
-        <v>9</v>
+      <c r="D57" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C58" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D58" t="s">
-        <v>22</v>
+      <c r="D58" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C59" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D59" t="s">
-        <v>25</v>
+      <c r="D59" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="7" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C60" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D60" t="s">
-        <v>28</v>
+      <c r="D60" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C61" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D61" t="s">
-        <v>31</v>
+      <c r="D61" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C62" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D62" t="s">
-        <v>34</v>
+      <c r="D62" s="14" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C63" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D63" t="s">
-        <v>37</v>
+      <c r="D63" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C64" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D64" t="s">
-        <v>40</v>
+      <c r="D64" s="14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C65" s="6" t="str">
         <f ca="1" t="shared" si="0"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D65" t="s">
-        <v>43</v>
+      <c r="D65" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C66" s="6" t="str">
         <f ca="1" t="shared" ref="C66:C129" si="1">IF(MID(A66,9,3)="120","SNMPTN",IF(MID(A66,9,3)="130","SBMPTN",IF(RAND()&lt;0.8,"Mandiri","Lainnya")))</f>
         <v>SBMPTN</v>
       </c>
-      <c r="D66" t="s">
-        <v>46</v>
+      <c r="D66" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C67" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D67" t="s">
-        <v>49</v>
+      <c r="D67" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C68" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D68" t="s">
-        <v>52</v>
+      <c r="D68" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="7" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C69" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D69" t="s">
-        <v>55</v>
+      <c r="D69" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C70" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D70" t="s">
-        <v>58</v>
+      <c r="D70" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="7" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C71" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D71" t="s">
-        <v>61</v>
+      <c r="D71" s="14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="7" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C72" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D72" t="s">
-        <v>64</v>
+      <c r="D72" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="7" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C73" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D73" t="s">
-        <v>67</v>
+      <c r="D73" s="14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="7" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C74" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D74" t="s">
-        <v>70</v>
+      <c r="D74" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="7" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C75" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D75" t="s">
-        <v>73</v>
+      <c r="D75" s="14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C76" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D76" t="s">
-        <v>76</v>
+      <c r="D76" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="7" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C77" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C78" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D78" t="s">
-        <v>6</v>
+      <c r="D78" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="7" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C79" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D79" t="s">
-        <v>6</v>
+      <c r="D79" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C80" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Lainnya</v>
       </c>
-      <c r="D80" t="s">
-        <v>14</v>
+      <c r="D80" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="7" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C81" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D81" t="s">
-        <v>17</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C82" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D82" t="s">
-        <v>9</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C83" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D83" t="s">
-        <v>22</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C84" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D84" t="s">
-        <v>25</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="7" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C85" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Lainnya</v>
       </c>
-      <c r="D85" t="s">
-        <v>28</v>
+      <c r="D85" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="7" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C86" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D86" t="s">
-        <v>31</v>
+      <c r="D86" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="7" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C87" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D87" t="s">
-        <v>34</v>
+      <c r="D87" s="14" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="7" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C88" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D88" t="s">
-        <v>37</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="7" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C89" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D89" t="s">
-        <v>40</v>
+      <c r="D89" s="14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C90" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D90" t="s">
-        <v>43</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C91" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D91" t="s">
-        <v>46</v>
+      <c r="D91" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C92" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D92" t="s">
-        <v>49</v>
+      <c r="D92" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C93" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D93" t="s">
-        <v>52</v>
+      <c r="D93" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="7" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C94" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D94" t="s">
-        <v>55</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="7" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C95" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D95" t="s">
-        <v>58</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="7" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C96" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D96" t="s">
-        <v>61</v>
+      <c r="D96" s="14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="7" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C97" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D97" t="s">
-        <v>64</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="7" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C98" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D98" t="s">
-        <v>67</v>
+      <c r="D98" s="14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="7" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C99" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D99" t="s">
-        <v>70</v>
+      <c r="D99" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="7" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C100" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D100" t="s">
-        <v>73</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="7" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C101" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D101" t="s">
-        <v>76</v>
+      <c r="D101" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="7" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C102" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="7" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C103" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D103" t="s">
-        <v>6</v>
+      <c r="D103" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="7" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C104" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D104" t="s">
-        <v>6</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="7" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C105" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D105" t="s">
-        <v>14</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D105" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="7" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C106" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>Mandiri</v>
       </c>
-      <c r="D106" t="s">
-        <v>17</v>
+      <c r="D106" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="7" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C107" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D107" t="s">
-        <v>9</v>
+      <c r="D107" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="7" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C108" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D108" t="s">
-        <v>22</v>
+      <c r="D108" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C109" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D109" t="s">
-        <v>25</v>
+      <c r="D109" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="7" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C110" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D110" t="s">
-        <v>28</v>
+      <c r="D110" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="7" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C111" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D111" t="s">
-        <v>31</v>
+      <c r="D111" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="7" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C112" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D112" t="s">
-        <v>34</v>
+      <c r="D112" s="14" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="7" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C113" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D113" t="s">
-        <v>37</v>
+      <c r="D113" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C114" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D114" t="s">
-        <v>40</v>
+      <c r="D114" s="14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="7" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C115" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D115" t="s">
-        <v>43</v>
+      <c r="D115" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="7" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C116" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SNMPTN</v>
       </c>
-      <c r="D116" t="s">
-        <v>46</v>
+      <c r="D116" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="7" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C117" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D117" t="s">
-        <v>49</v>
+      <c r="D117" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="7" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C118" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D118" t="s">
-        <v>52</v>
+      <c r="D118" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="7" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C119" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D119" t="s">
-        <v>55</v>
+      <c r="D119" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="7" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C120" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D120" t="s">
-        <v>58</v>
+      <c r="D120" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="7" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C121" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D121" t="s">
-        <v>61</v>
+      <c r="D121" s="14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="7" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C122" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D122" t="s">
-        <v>64</v>
+      <c r="D122" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="7" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C123" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D123" t="s">
-        <v>67</v>
+      <c r="D123" s="14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="15" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C124" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D124" t="s">
-        <v>70</v>
+      <c r="D124" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="7" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C125" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D125" t="s">
-        <v>73</v>
+      <c r="D125" s="14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="7" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C126" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D126" t="s">
-        <v>76</v>
+      <c r="D126" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="7" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C127" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="7" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C128" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D128" t="s">
-        <v>6</v>
+      <c r="D128" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="7" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C129" s="6" t="str">
         <f ca="1" t="shared" si="1"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D129" t="s">
-        <v>6</v>
+      <c r="D129" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="7" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C130" s="6" t="str">
         <f ca="1" t="shared" ref="C130:C161" si="2">IF(MID(A130,9,3)="120","SNMPTN",IF(MID(A130,9,3)="130","SBMPTN",IF(RAND()&lt;0.8,"Mandiri","Lainnya")))</f>
         <v>SBMPTN</v>
       </c>
-      <c r="D130" t="s">
-        <v>14</v>
+      <c r="D130" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="7" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C131" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D131" t="s">
-        <v>17</v>
+      <c r="D131" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="7" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C132" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D132" t="s">
-        <v>9</v>
+      <c r="D132" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="7" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C133" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D133" t="s">
-        <v>22</v>
+      <c r="D133" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="7" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C134" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>SBMPTN</v>
       </c>
-      <c r="D134" t="s">
-        <v>25</v>
+      <c r="D134" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="7" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C135" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D135" t="s">
-        <v>28</v>
+      <c r="D135" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="7" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C136" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D136" t="s">
-        <v>31</v>
+      <c r="D136" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="7" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C137" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D137" t="s">
-        <v>34</v>
+      <c r="D137" s="14" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="7" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C138" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D138" t="s">
-        <v>37</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D138" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="7" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C139" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D139" t="s">
-        <v>40</v>
+      <c r="D139" s="14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="7" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C140" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D140" t="s">
-        <v>43</v>
+      <c r="D140" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="7" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C141" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D141" t="s">
-        <v>46</v>
+      <c r="D141" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="7" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C142" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D142" t="s">
-        <v>49</v>
+      <c r="D142" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="7" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C143" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Lainnya</v>
       </c>
-      <c r="D143" t="s">
-        <v>52</v>
+      <c r="D143" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="7" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C144" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D144" t="s">
-        <v>55</v>
+      <c r="D144" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="7" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C145" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D145" t="s">
-        <v>58</v>
+      <c r="D145" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="7" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C146" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D146" t="s">
-        <v>61</v>
+      <c r="D146" s="14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="7" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C147" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Lainnya</v>
       </c>
-      <c r="D147" t="s">
-        <v>64</v>
+      <c r="D147" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="7" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C148" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D148" t="s">
-        <v>67</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D148" s="14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="7" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C149" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D149" t="s">
-        <v>70</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D149" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="7" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C150" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D150" t="s">
-        <v>73</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D150" s="14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="7" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C151" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D151" t="s">
-        <v>76</v>
+      <c r="D151" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="7" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C152" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D152" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="7" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C153" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D153" t="s">
-        <v>6</v>
+      <c r="D153" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="7" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C154" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D154" t="s">
-        <v>6</v>
+      <c r="D154" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="7" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="C155" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D155" t="s">
-        <v>14</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D155" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="7" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C156" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>Mandiri</v>
-      </c>
-      <c r="D156" t="s">
-        <v>17</v>
+        <v>Lainnya</v>
+      </c>
+      <c r="D156" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="7" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C157" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D157" t="s">
-        <v>9</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D157" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="7" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="C158" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D158" t="s">
-        <v>22</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D158" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="7" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C159" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
-        <v>Lainnya</v>
-      </c>
-      <c r="D159" t="s">
-        <v>25</v>
+        <v>Mandiri</v>
+      </c>
+      <c r="D159" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="7" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C160" s="6" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D160" t="s">
-        <v>25</v>
+      <c r="D160" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="7" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C161" s="10" t="str">
         <f ca="1" t="shared" si="2"/>
         <v>Mandiri</v>
       </c>
-      <c r="D161" s="11" t="s">
-        <v>31</v>
+      <c r="D161" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="162" spans="1:4">
-      <c r="A162" s="12"/>
-      <c r="B162" s="12"/>
-      <c r="C162" s="13"/>
-      <c r="D162" s="14"/>
+      <c r="A162" s="11"/>
+      <c r="B162" s="11"/>
+      <c r="C162" s="12"/>
+      <c r="D162" s="13"/>
     </row>
     <row r="163" spans="1:4">
-      <c r="A163" s="12"/>
-      <c r="B163" s="12"/>
-      <c r="C163" s="13"/>
-      <c r="D163" s="14"/>
+      <c r="A163" s="11"/>
+      <c r="B163" s="11"/>
+      <c r="C163" s="12"/>
+      <c r="D163" s="13"/>
     </row>
     <row r="164" spans="1:4">
-      <c r="A164" s="12"/>
-      <c r="B164" s="12"/>
-      <c r="C164" s="13"/>
-      <c r="D164" s="14"/>
+      <c r="A164" s="11"/>
+      <c r="B164" s="11"/>
+      <c r="C164" s="12"/>
+      <c r="D164" s="13"/>
     </row>
     <row r="165" spans="1:4">
-      <c r="A165" s="12"/>
-      <c r="B165" s="12"/>
-      <c r="C165" s="13"/>
-      <c r="D165" s="14"/>
+      <c r="A165" s="11"/>
+      <c r="B165" s="11"/>
+      <c r="C165" s="12"/>
+      <c r="D165" s="13"/>
     </row>
     <row r="166" spans="1:4">
-      <c r="A166" s="12"/>
-      <c r="B166" s="12"/>
-      <c r="C166" s="13"/>
-      <c r="D166" s="14"/>
+      <c r="A166" s="11"/>
+      <c r="B166" s="11"/>
+      <c r="C166" s="12"/>
+      <c r="D166" s="13"/>
     </row>
     <row r="167" spans="1:4">
-      <c r="A167" s="12"/>
-      <c r="B167" s="12"/>
-      <c r="C167" s="13"/>
-      <c r="D167" s="14"/>
+      <c r="A167" s="11"/>
+      <c r="B167" s="11"/>
+      <c r="C167" s="12"/>
+      <c r="D167" s="13"/>
     </row>
     <row r="168" spans="1:4">
-      <c r="A168" s="12"/>
-      <c r="B168" s="12"/>
-      <c r="C168" s="13"/>
-      <c r="D168" s="14"/>
+      <c r="A168" s="11"/>
+      <c r="B168" s="11"/>
+      <c r="C168" s="12"/>
+      <c r="D168" s="13"/>
     </row>
     <row r="169" spans="1:4">
-      <c r="A169" s="12"/>
-      <c r="B169" s="12"/>
-      <c r="C169" s="13"/>
-      <c r="D169" s="14"/>
+      <c r="A169" s="11"/>
+      <c r="B169" s="11"/>
+      <c r="C169" s="12"/>
+      <c r="D169" s="13"/>
     </row>
     <row r="170" spans="1:4">
-      <c r="A170" s="12"/>
-      <c r="B170" s="12"/>
-      <c r="C170" s="13"/>
-      <c r="D170" s="14"/>
+      <c r="A170" s="11"/>
+      <c r="B170" s="11"/>
+      <c r="C170" s="12"/>
+      <c r="D170" s="13"/>
     </row>
     <row r="171" spans="1:4">
-      <c r="A171" s="12"/>
-      <c r="B171" s="12"/>
-      <c r="C171" s="13"/>
-      <c r="D171" s="14"/>
+      <c r="A171" s="11"/>
+      <c r="B171" s="11"/>
+      <c r="C171" s="12"/>
+      <c r="D171" s="13"/>
     </row>
     <row r="172" spans="1:4">
-      <c r="A172" s="12"/>
-      <c r="B172" s="12"/>
-      <c r="C172" s="13"/>
-      <c r="D172" s="14"/>
+      <c r="A172" s="11"/>
+      <c r="B172" s="11"/>
+      <c r="C172" s="12"/>
+      <c r="D172" s="13"/>
     </row>
     <row r="173" spans="1:4">
-      <c r="A173" s="12"/>
-      <c r="B173" s="12"/>
-      <c r="C173" s="13"/>
-      <c r="D173" s="14"/>
+      <c r="A173" s="11"/>
+      <c r="B173" s="11"/>
+      <c r="C173" s="12"/>
+      <c r="D173" s="13"/>
     </row>
     <row r="174" spans="1:4">
-      <c r="A174" s="12"/>
-      <c r="B174" s="12"/>
-      <c r="C174" s="13"/>
-      <c r="D174" s="14"/>
+      <c r="A174" s="11"/>
+      <c r="B174" s="11"/>
+      <c r="C174" s="12"/>
+      <c r="D174" s="13"/>
     </row>
     <row r="175" spans="1:4">
-      <c r="A175" s="12"/>
-      <c r="B175" s="12"/>
-      <c r="C175" s="13"/>
-      <c r="D175" s="14"/>
+      <c r="A175" s="11"/>
+      <c r="B175" s="11"/>
+      <c r="C175" s="12"/>
+      <c r="D175" s="13"/>
     </row>
     <row r="176" spans="1:4">
-      <c r="A176" s="12"/>
-      <c r="B176" s="12"/>
-      <c r="C176" s="13"/>
-      <c r="D176" s="14"/>
+      <c r="A176" s="11"/>
+      <c r="B176" s="11"/>
+      <c r="C176" s="12"/>
+      <c r="D176" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4737,36 +4749,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>